<commit_message>
c/v gets me the all the table in the page.
</commit_message>
<xml_diff>
--- a/ARCC/ARCC__sec_filing_links.xlsx
+++ b/ARCC/ARCC__sec_filing_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fuadhassan/Desktop/BDC_RA/ARCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04D65F8-7943-E143-A829-65916BA97A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549EBE49-08C0-B14A-A760-A91FAC7EB06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AF42AFBB-B051-004D-958D-77C93AF86980}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{AF42AFBB-B051-004D-958D-77C93AF86980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,8 +604,8 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,64 +640,64 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>45132</v>
+        <v>40486</v>
       </c>
       <c r="D2" s="2">
-        <v>45107</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
+        <v>40451</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>45041</v>
+        <v>40603</v>
       </c>
       <c r="D3" s="2">
-        <v>45016</v>
+        <v>40543</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>45016</v>
+        <v>40666</v>
       </c>
       <c r="D4" s="2">
-        <v>44926</v>
+        <v>40633</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
-        <v>44964</v>
+        <v>40759</v>
       </c>
       <c r="D5" s="2">
-        <v>44926</v>
+        <v>40724</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -708,30 +708,30 @@
         <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>44859</v>
+        <v>40855</v>
       </c>
       <c r="D6" s="2">
-        <v>44834</v>
+        <v>40816</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>44768</v>
+        <v>40967</v>
       </c>
       <c r="D7" s="2">
-        <v>44742</v>
+        <v>40908</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -742,30 +742,30 @@
         <v>10</v>
       </c>
       <c r="C8" s="2">
-        <v>44677</v>
+        <v>41037</v>
       </c>
       <c r="D8" s="2">
-        <v>44651</v>
+        <v>40999</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2">
-        <v>44601</v>
+        <v>41128</v>
       </c>
       <c r="D9" s="2">
-        <v>44561</v>
+        <v>41090</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -776,30 +776,30 @@
         <v>10</v>
       </c>
       <c r="C10" s="2">
-        <v>44495</v>
+        <v>41218</v>
       </c>
       <c r="D10" s="2">
-        <v>44469</v>
+        <v>41182</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2">
-        <v>44405</v>
+        <v>41332</v>
       </c>
       <c r="D11" s="2">
-        <v>44377</v>
+        <v>41274</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -810,64 +810,64 @@
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>44314</v>
+        <v>41401</v>
       </c>
       <c r="D12" s="2">
-        <v>44286</v>
+        <v>41364</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2">
-        <v>44260</v>
+        <v>41492</v>
       </c>
       <c r="D13" s="2">
-        <v>44196</v>
+        <v>41455</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
-        <v>44237</v>
+        <v>41583</v>
       </c>
       <c r="D14" s="2">
-        <v>44196</v>
+        <v>41547</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
-        <v>44131</v>
+        <v>41696</v>
       </c>
       <c r="D15" s="2">
-        <v>44104</v>
+        <v>41639</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -878,13 +878,13 @@
         <v>10</v>
       </c>
       <c r="C16" s="2">
-        <v>44047</v>
+        <v>41765</v>
       </c>
       <c r="D16" s="2">
-        <v>44012</v>
+        <v>41729</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -895,47 +895,47 @@
         <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>43956</v>
+        <v>41856</v>
       </c>
       <c r="D17" s="2">
-        <v>43921</v>
+        <v>41820</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2">
-        <v>43873</v>
+        <v>41947</v>
       </c>
       <c r="D18" s="2">
-        <v>43830</v>
+        <v>41912</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C19" s="2">
-        <v>43768</v>
+        <v>42061</v>
       </c>
       <c r="D19" s="2">
-        <v>43738</v>
+        <v>42004</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -946,13 +946,13 @@
         <v>10</v>
       </c>
       <c r="C20" s="2">
-        <v>43676</v>
+        <v>42128</v>
       </c>
       <c r="D20" s="2">
-        <v>43646</v>
+        <v>42094</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -963,47 +963,47 @@
         <v>10</v>
       </c>
       <c r="C21" s="2">
-        <v>43585</v>
+        <v>42220</v>
       </c>
       <c r="D21" s="2">
-        <v>43555</v>
+        <v>42185</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C22" s="2">
-        <v>43508</v>
+        <v>42312</v>
       </c>
       <c r="D22" s="2">
-        <v>43465</v>
+        <v>42277</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2">
-        <v>43404</v>
+        <v>42424</v>
       </c>
       <c r="D23" s="2">
-        <v>43373</v>
+        <v>42369</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1014,13 +1014,13 @@
         <v>10</v>
       </c>
       <c r="C24" s="2">
-        <v>43313</v>
+        <v>42494</v>
       </c>
       <c r="D24" s="2">
-        <v>43281</v>
+        <v>42460</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1031,47 +1031,47 @@
         <v>10</v>
       </c>
       <c r="C25" s="2">
-        <v>43222</v>
+        <v>42585</v>
       </c>
       <c r="D25" s="2">
-        <v>43190</v>
+        <v>42551</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C26" s="2">
-        <v>43144</v>
+        <v>42676</v>
       </c>
       <c r="D26" s="2">
-        <v>43100</v>
+        <v>42643</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2">
-        <v>43041</v>
+        <v>42788</v>
       </c>
       <c r="D27" s="2">
-        <v>43008</v>
+        <v>42735</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1082,13 +1082,13 @@
         <v>10</v>
       </c>
       <c r="C28" s="2">
-        <v>42949</v>
+        <v>42858</v>
       </c>
       <c r="D28" s="2">
-        <v>42916</v>
+        <v>42825</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1099,47 +1099,47 @@
         <v>10</v>
       </c>
       <c r="C29" s="2">
-        <v>42858</v>
+        <v>42949</v>
       </c>
       <c r="D29" s="2">
-        <v>42825</v>
+        <v>42916</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C30" s="2">
-        <v>42788</v>
+        <v>43041</v>
       </c>
       <c r="D30" s="2">
-        <v>42735</v>
+        <v>43008</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C31" s="2">
-        <v>42676</v>
+        <v>43144</v>
       </c>
       <c r="D31" s="2">
-        <v>42643</v>
+        <v>43100</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1150,13 +1150,13 @@
         <v>10</v>
       </c>
       <c r="C32" s="2">
-        <v>42585</v>
+        <v>43222</v>
       </c>
       <c r="D32" s="2">
-        <v>42551</v>
+        <v>43190</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1167,47 +1167,47 @@
         <v>10</v>
       </c>
       <c r="C33" s="2">
-        <v>42494</v>
+        <v>43313</v>
       </c>
       <c r="D33" s="2">
-        <v>42460</v>
+        <v>43281</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C34" s="2">
-        <v>42424</v>
+        <v>43404</v>
       </c>
       <c r="D34" s="2">
-        <v>42369</v>
+        <v>43373</v>
       </c>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C35" s="2">
-        <v>42312</v>
+        <v>43508</v>
       </c>
       <c r="D35" s="2">
-        <v>42277</v>
+        <v>43465</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1218,13 +1218,13 @@
         <v>10</v>
       </c>
       <c r="C36" s="2">
-        <v>42220</v>
+        <v>43585</v>
       </c>
       <c r="D36" s="2">
-        <v>42185</v>
+        <v>43555</v>
       </c>
       <c r="E36" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1235,47 +1235,47 @@
         <v>10</v>
       </c>
       <c r="C37" s="2">
-        <v>42128</v>
+        <v>43676</v>
       </c>
       <c r="D37" s="2">
-        <v>42094</v>
+        <v>43646</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C38" s="2">
-        <v>42061</v>
+        <v>43768</v>
       </c>
       <c r="D38" s="2">
-        <v>42004</v>
+        <v>43738</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C39" s="2">
-        <v>41947</v>
+        <v>43873</v>
       </c>
       <c r="D39" s="2">
-        <v>41912</v>
+        <v>43830</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1286,13 +1286,13 @@
         <v>10</v>
       </c>
       <c r="C40" s="2">
-        <v>41856</v>
+        <v>43956</v>
       </c>
       <c r="D40" s="2">
-        <v>41820</v>
+        <v>43921</v>
       </c>
       <c r="E40" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1303,64 +1303,64 @@
         <v>10</v>
       </c>
       <c r="C41" s="2">
-        <v>41765</v>
+        <v>44047</v>
       </c>
       <c r="D41" s="2">
-        <v>41729</v>
+        <v>44012</v>
       </c>
       <c r="E41" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C42" s="2">
-        <v>41696</v>
+        <v>44131</v>
       </c>
       <c r="D42" s="2">
-        <v>41639</v>
+        <v>44104</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C43" s="2">
-        <v>41583</v>
+        <v>44260</v>
       </c>
       <c r="D43" s="2">
-        <v>41547</v>
+        <v>44196</v>
       </c>
       <c r="E43" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C44" s="2">
-        <v>41492</v>
+        <v>44237</v>
       </c>
       <c r="D44" s="2">
-        <v>41455</v>
+        <v>44196</v>
       </c>
       <c r="E44" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1371,30 +1371,30 @@
         <v>10</v>
       </c>
       <c r="C45" s="2">
-        <v>41401</v>
+        <v>44314</v>
       </c>
       <c r="D45" s="2">
-        <v>41364</v>
+        <v>44286</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C46" s="2">
-        <v>41332</v>
+        <v>44405</v>
       </c>
       <c r="D46" s="2">
-        <v>41274</v>
+        <v>44377</v>
       </c>
       <c r="E46" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1405,30 +1405,30 @@
         <v>10</v>
       </c>
       <c r="C47" s="2">
-        <v>41218</v>
+        <v>44495</v>
       </c>
       <c r="D47" s="2">
-        <v>41182</v>
+        <v>44469</v>
       </c>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C48" s="2">
-        <v>41128</v>
+        <v>44601</v>
       </c>
       <c r="D48" s="2">
-        <v>41090</v>
+        <v>44561</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1439,30 +1439,30 @@
         <v>10</v>
       </c>
       <c r="C49" s="2">
-        <v>41037</v>
+        <v>44677</v>
       </c>
       <c r="D49" s="2">
-        <v>40999</v>
+        <v>44651</v>
       </c>
       <c r="E49" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C50" s="2">
-        <v>40967</v>
+        <v>44768</v>
       </c>
       <c r="D50" s="2">
-        <v>40908</v>
+        <v>44742</v>
       </c>
       <c r="E50" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1473,64 +1473,64 @@
         <v>10</v>
       </c>
       <c r="C51" s="2">
-        <v>40855</v>
+        <v>44859</v>
       </c>
       <c r="D51" s="2">
-        <v>40816</v>
+        <v>44834</v>
       </c>
       <c r="E51" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C52" s="2">
-        <v>40759</v>
+        <v>45016</v>
       </c>
       <c r="D52" s="2">
-        <v>40724</v>
+        <v>44926</v>
       </c>
       <c r="E52" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C53" s="2">
-        <v>40666</v>
+        <v>44964</v>
       </c>
       <c r="D53" s="2">
-        <v>40633</v>
+        <v>44926</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C54" s="2">
-        <v>40603</v>
+        <v>45041</v>
       </c>
       <c r="D54" s="2">
-        <v>40543</v>
+        <v>45016</v>
       </c>
       <c r="E54" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1541,18 +1541,21 @@
         <v>10</v>
       </c>
       <c r="C55" s="2">
-        <v>40486</v>
+        <v>45132</v>
       </c>
       <c r="D55" s="2">
-        <v>40451</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>63</v>
+        <v>45107</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E55">
+    <sortCondition ref="D1:D55"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="E55" r:id="rId1" xr:uid="{43C207E7-9CD4-034E-935F-3E309E755705}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{43C207E7-9CD4-034E-935F-3E309E755705}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>